<commit_message>
wrote insert code from df to db
</commit_message>
<xml_diff>
--- a/contact_details.xlsx
+++ b/contact_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\27722\Desktop\pd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8D02AB-F5A6-4C1F-942B-2BBCA74B3EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5BD90C-FC99-435D-80C7-E73A99F267DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{807C83B1-584F-4EF8-BF4E-18C308A34833}"/>
   </bookViews>
@@ -81,9 +81,6 @@
     <t>Wits University</t>
   </si>
   <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>South Africa</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>Accountant</t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
     <t>0720134278</t>
   </si>
   <si>
@@ -124,6 +118,12 @@
   </si>
   <si>
     <t>10/3/1997</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>male</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -530,7 +530,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>12</v>
@@ -542,62 +542,62 @@
         <v>14</v>
       </c>
       <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
         <v>29</v>
       </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
-        <v>25</v>
-      </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>